<commit_message>
-Implemented get_year_prompt function -Updated tax rates for year 2021-2022
</commit_message>
<xml_diff>
--- a/tax_rates.xlsx
+++ b/tax_rates.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\charm\TaxCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C028E84-743C-4F7A-94EE-C71987D1FAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843F7400-1216-4CC1-9C4F-B4DE9D7B45B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="675" windowWidth="18900" windowHeight="9420" xr2:uid="{A574C2AF-53E6-49DD-986F-C9179E9E3E4A}"/>
+    <workbookView xWindow="3480" yWindow="675" windowWidth="18900" windowHeight="9420" activeTab="1" xr2:uid="{A574C2AF-53E6-49DD-986F-C9179E9E3E4A}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-2021" sheetId="1" r:id="rId1"/>
+    <sheet name="2021-2022" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Tax_Bracket</t>
   </si>
@@ -404,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1C1575-A028-4C1D-B1AD-54E62D0A4B88}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -521,4 +522,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA49DCF-0DBD-44B8-A857-93DE9F2D4E84}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.46484375" customWidth="1"/>
+    <col min="2" max="2" width="9.86328125" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" customWidth="1"/>
+    <col min="5" max="5" width="16.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>18200</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>18201</v>
+      </c>
+      <c r="C3">
+        <v>45000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>45001</v>
+      </c>
+      <c r="C4">
+        <v>120000</v>
+      </c>
+      <c r="D4">
+        <v>5092</v>
+      </c>
+      <c r="E4">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>120001</v>
+      </c>
+      <c r="C5">
+        <v>180000</v>
+      </c>
+      <c r="D5">
+        <v>29467</v>
+      </c>
+      <c r="E5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>180001</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>51667</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>